<commit_message>
Before the octo is taken for weekend testing
</commit_message>
<xml_diff>
--- a/Octoscope_Configuration.xlsx
+++ b/Octoscope_Configuration.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t xml:space="preserve">TEST NAME</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t xml:space="preserve">PAL6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAL6_Automation-2</t>
   </si>
   <si>
     <t xml:space="preserve">Testing Profile- not to use for testing platforms </t>
@@ -126,7 +129,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -147,11 +150,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="28"/>
@@ -265,16 +263,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -282,11 +276,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -298,27 +296,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -402,7 +396,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -484,8 +478,8 @@
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
+      <c r="A3" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -522,19 +516,19 @@
     <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
+      <c r="A25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -569,117 +563,117 @@
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>20</v>
+      <c r="B7" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>21</v>
+      <c r="B8" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>22</v>
+      <c r="B9" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9" t="n">
+      <c r="B10" s="8" t="n">
         <v>12345678</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>23</v>
+      <c r="A15" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>24</v>
+      <c r="B17" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>28</v>
+      <c r="B20" s="12" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="12" t="n">
+      <c r="B21" s="11" t="n">
         <v>12345678</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="11" t="s">
+      <c r="A22" s="9" t="s">
         <v>30</v>
       </c>
+      <c r="B22" s="10" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>31</v>
+      <c r="A23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
JSON completed, now GUI
</commit_message>
<xml_diff>
--- a/Octoscope_Configuration.xlsx
+++ b/Octoscope_Configuration.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t xml:space="preserve">TEST NAME</t>
   </si>
@@ -62,7 +62,7 @@
     <t xml:space="preserve">MH_5G</t>
   </si>
   <si>
-    <t xml:space="preserve">BANDWIDTH_80_ADAPT</t>
+    <t xml:space="preserve">BANDWIDTH_160_ADAPT</t>
   </si>
   <si>
     <t xml:space="preserve">RADIO_5</t>
@@ -129,12 +129,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+  <fonts count="25">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -152,23 +151,103 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCE181E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="28"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -176,7 +255,6 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -185,20 +263,17 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="24"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="24"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -206,15 +281,56 @@
       <sz val="24"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FFCE181E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -229,7 +345,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -237,8 +353,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -262,8 +393,59 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -272,73 +454,94 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -350,7 +553,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -366,7 +569,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -379,7 +582,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFCE181E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -396,7 +599,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -445,90 +648,137 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="G2" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="I2" s="0" t="n">
         <v>12345678</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>12345678</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="G4" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="I4" s="0" t="n">
         <v>12345678</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J4" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2"/>
+    </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -563,116 +813,116 @@
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="n">
+      <c r="B10" s="9" t="n">
         <v>12345678</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="11" t="n">
+      <c r="B21" s="12" t="n">
         <v>12345678</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="11" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
workin with GUI and automation restart
</commit_message>
<xml_diff>
--- a/Octoscope_Configuration.xlsx
+++ b/Octoscope_Configuration.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t xml:space="preserve">TEST NAME</t>
   </si>
@@ -72,12 +72,6 @@
   </si>
   <si>
     <t xml:space="preserve">PAL6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAL6_Automation-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testing Profile- not to use for testing platforms </t>
   </si>
   <si>
     <t xml:space="preserve">Bandwidth</t>
@@ -129,11 +123,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -151,103 +146,23 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCE181E"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="28"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -255,6 +170,7 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -263,17 +179,20 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="24"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="24"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -281,56 +200,15 @@
       <sz val="24"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFCE181E"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -345,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -353,23 +231,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -393,59 +256,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -454,94 +266,69 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -553,7 +340,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -569,7 +356,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -582,7 +369,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FFCE181E"/>
+      <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -596,10 +383,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -616,7 +403,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -648,8 +435,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -680,8 +467,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -712,9 +499,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
+    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
@@ -744,46 +531,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A25:K25"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -802,7 +550,7 @@
   <dimension ref="A4:B24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="A4 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -813,117 +561,117 @@
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="6" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="7" t="s">
+    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="8" t="s">
+    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+    <row r="17" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="B20" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9" t="n">
+      <c r="B21" s="10" t="n">
         <v>12345678</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
+    <row r="22" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="13" t="s">
+      <c r="B22" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="12" t="n">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
+    <row r="23" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>